<commit_message>
basic xgboost urolithiasis for binary data
</commit_message>
<xml_diff>
--- a/static/mock/urolithiasis/Stones_Train.xlsx
+++ b/static/mock/urolithiasis/Stones_Train.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgramProj/ChemML/static/mock/urolithiasis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70052A6-9A01-6F44-BE00-80BBDFAEDE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8539F717-CCCB-6F43-AD9F-AD11AAEE4F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="катя" sheetId="1" r:id="rId1"/>
@@ -778,7 +778,7 @@
   <dimension ref="A1:BN75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="BL68" sqref="BL68"/>
+      <selection activeCell="BJ67" sqref="BJ67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="BJ4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.15">
@@ -1670,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="BJ5">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
@@ -2906,7 +2906,7 @@
         <v>2</v>
       </c>
       <c r="BJ12">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
@@ -3044,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="BJ13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
@@ -3578,7 +3578,7 @@
         <v>3</v>
       </c>
       <c r="BJ16">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.15">
@@ -3628,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="BJ17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.15">
@@ -4470,7 +4470,7 @@
         <v>2</v>
       </c>
       <c r="BJ22">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.15">
@@ -9267,7 +9267,7 @@
         <v>3</v>
       </c>
       <c r="BJ50" s="23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BK50" s="23"/>
       <c r="BL50" s="23"/>
@@ -9443,7 +9443,7 @@
         <v>2</v>
       </c>
       <c r="BJ51" s="23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BK51" s="23"/>
       <c r="BL51" s="23"/>
@@ -10327,7 +10327,7 @@
         <v>3</v>
       </c>
       <c r="BJ56" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BK56" s="23"/>
       <c r="BL56" s="23"/>
@@ -11693,7 +11693,7 @@
         <v>3</v>
       </c>
       <c r="BJ64" s="23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BK64" s="23"/>
       <c r="BL64" s="23"/>
@@ -13251,7 +13251,7 @@
         <v>2</v>
       </c>
       <c r="BJ74">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:64" x14ac:dyDescent="0.15">
@@ -13358,7 +13358,7 @@
         <v>1</v>
       </c>
       <c r="BJ75">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>